<commit_message>
work on coding parser began... Should I redo my prints to listing file via a linked list and then print them afterward so syntax error and semantic errors are together with the line numbers? need to consult someone about this
</commit_message>
<xml_diff>
--- a/WrittenWork/ParseTable.xlsx
+++ b/WrittenWork/ParseTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelcollett/Compilerv2/Compiler/WrittenWork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E989352B-5D99-2E4F-A1C0-D31A3CC4A3BD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D510F484-D932-0D4C-90A2-1961F61F24F1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="19160" windowHeight="21600" xr2:uid="{9F8CB507-561A-604A-A82F-23B2F5C132D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="18000" xr2:uid="{9F8CB507-561A-604A-A82F-23B2F5C132D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E703A7-E904-2247-9A43-BF23FFACE658}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>